<commit_message>
Elimina antiguos EC y agrega nuevos y modifica Antigua BD
</commit_message>
<xml_diff>
--- a/Data/EC/CC-1001968539.xlsx
+++ b/Data/EC/CC-1001968539.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\NIYARAKY\MACROS AJUSTADAS\2- MACRO COMFENALCO CARTAGENA ACTUALIZACION\Estados De Cuenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8780BAA5-9B89-4D2B-AE7B-B82109493343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C17BED1F-C715-4E57-AB12-D006BF6B32B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E7B05599-ADEB-464C-B8A7-8A4C6FF1BA19}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6427F2A4-9214-4562-ADB6-4FD034891E88}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -185,22 +185,22 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -394,29 +394,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,19 +435,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -500,7 +506,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EABC6339-3C90-0F08-418A-A6267C429286}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5012321C-89D4-D475-0615-B7DEDC4341FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -851,7 +857,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1C27AB-1F65-404A-91B8-864EA0E8AF43}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B14E666-FE1D-447B-84B3-B2794B14FC7E}">
   <dimension ref="B2:J28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
@@ -874,49 +880,49 @@
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="3"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
     </row>
     <row r="6" spans="2:10" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
@@ -924,7 +930,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="27"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="6" t="s">
         <v>7</v>
       </c>
@@ -940,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="27"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="6">
         <v>1001968539</v>
       </c>
@@ -956,7 +962,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="27"/>
+      <c r="D11" s="29"/>
       <c r="E11" s="7">
         <v>280000</v>
       </c>
@@ -1025,18 +1031,18 @@
       <c r="D16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="19">
         <v>40000</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="19">
         <v>1000000</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="21"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
@@ -1048,18 +1054,18 @@
       <c r="D17" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="19">
         <v>40000</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="19">
         <v>1000000</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="15" t="s">
@@ -1071,18 +1077,18 @@
       <c r="D18" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="19">
         <v>40000</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="19">
         <v>1000000</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
@@ -1094,18 +1100,18 @@
       <c r="D19" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="19">
         <v>40000</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="19">
         <v>1000000</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="15" t="s">
@@ -1117,18 +1123,18 @@
       <c r="D20" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="19">
         <v>40000</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="19">
         <v>1000000</v>
       </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B21" s="15" t="s">
@@ -1140,47 +1146,47 @@
       <c r="D21" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="19">
         <v>40000</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="19">
         <v>1000000</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="24">
+      <c r="F22" s="26">
         <v>40000</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="26">
         <v>1000000</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="26"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="28"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="32"/>
+      <c r="C27" s="34"/>
       <c r="H27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1188,10 +1194,10 @@
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="32"/>
+      <c r="C28" s="34"/>
       <c r="H28" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>